<commit_message>
Imrpoved sample titles & IDs
</commit_message>
<xml_diff>
--- a/extras/sample-form/Sample form - Create Google Calendar event field plug-in (advanced).xlsx
+++ b/extras/sample-form/Sample form - Create Google Calendar event field plug-in (advanced).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acooper/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acooper/Google Drive/GitHub/create-google-event/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CB2A4F-D0EF-5346-AD53-DBF0F1D836DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3DBB47-D30F-1545-B5AA-E17FC72E0E4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8840" yWindow="4700" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5080" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -2600,12 +2600,6 @@
     <t>min=0.25;max=2</t>
   </si>
   <si>
-    <t>Sample form - Create Google Calendar event field plug-in</t>
-  </si>
-  <si>
-    <t>google_calendar_plug-in_sample</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -3104,6 +3098,12 @@
 &lt;p&gt;&lt;strong&gt;Note:&lt;/strong&gt; If you're testing on web forms, keep in mind that times will be displayed in UTC format (server time). If you will be working with web forms, see &lt;a href="Welcome%20to this SurveyCTO sample form for the create-google-calendar event field plug-in.  While this sample form will walk you through all parameters, you only need to specify the title and start_time parameters.  In reality, you will want users to specify as few of the necessary parameters as possible. This form is mostly to help you understand your options with the create-google-calendar field plug-in.  Select Next to continue." target="_blank" rel="noopener"&gt;this article&lt;/a&gt; for advice on how to adjust.&lt;/p&gt;
 &lt;p&gt;&amp;nbsp;&lt;/p&gt;
 &lt;p&gt;Select &lt;em&gt;Next&lt;/em&gt; to continue.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>google_calendar_plug-in_adv_sample</t>
+  </si>
+  <si>
+    <t>Sample form - Create Google Calendar event field plug-in (advanced)</t>
   </si>
 </sst>
 </file>
@@ -6418,8 +6418,8 @@
   <dimension ref="A1:W40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6620,44 +6620,44 @@
         <v>42</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="9" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="119" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>402</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="H13" s="11" t="s">
         <v>391</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>374</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>375</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>404</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>390</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>392</v>
-      </c>
-      <c r="H13" s="11" t="s">
+      <c r="K13" s="9" t="s">
         <v>393</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="17" x14ac:dyDescent="0.2">
@@ -6665,16 +6665,16 @@
         <v>96</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="34" x14ac:dyDescent="0.2">
@@ -6682,19 +6682,19 @@
         <v>306</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="34" x14ac:dyDescent="0.2">
@@ -6702,16 +6702,16 @@
         <v>118</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>401</v>
+      </c>
+      <c r="I16" s="9" t="s">
         <v>398</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>412</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>403</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6719,13 +6719,13 @@
         <v>132</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="I17" s="9" t="s">
         <v>399</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>413</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6733,13 +6733,13 @@
         <v>148</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -6747,19 +6747,19 @@
         <v>118</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -6767,19 +6767,19 @@
         <v>132</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6787,13 +6787,13 @@
         <v>148</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -6801,16 +6801,16 @@
         <v>96</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="119" x14ac:dyDescent="0.2">
@@ -6818,16 +6818,16 @@
         <v>96</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="102" x14ac:dyDescent="0.2">
@@ -6835,16 +6835,16 @@
         <v>42</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>420</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>423</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>422</v>
-      </c>
       <c r="I24" s="9" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -6852,13 +6852,13 @@
         <v>163</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -6866,7 +6866,7 @@
         <v>148</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="N26" s="9" t="s">
         <v>320</v>
@@ -6877,16 +6877,16 @@
         <v>96</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -6894,7 +6894,7 @@
         <v>164</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -6902,33 +6902,33 @@
         <v>148</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="209" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>517</v>
+      </c>
+      <c r="D30" s="11" t="s">
         <v>430</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>433</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>519</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>432</v>
-      </c>
       <c r="I30" s="9" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="68" x14ac:dyDescent="0.2">
@@ -6936,13 +6936,13 @@
         <v>96</v>
       </c>
       <c r="B31" s="9" t="s">
+        <v>447</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="I31" s="9" t="s">
         <v>449</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>450</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -6950,30 +6950,30 @@
         <v>148</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="136" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>453</v>
+      </c>
+      <c r="C33" s="10" t="s">
         <v>454</v>
       </c>
-      <c r="B33" s="9" t="s">
-        <v>455</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>456</v>
-      </c>
       <c r="I33" s="9" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
@@ -6981,41 +6981,41 @@
         <v>148</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="119" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="I35" s="9" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="153" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>496</v>
+      </c>
+      <c r="I36" s="9" t="s">
         <v>485</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>493</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -7023,13 +7023,13 @@
         <v>100</v>
       </c>
       <c r="B37" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>497</v>
+      </c>
+      <c r="I37" s="9" t="s">
         <v>494</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>499</v>
-      </c>
-      <c r="I37" s="9" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -7037,16 +7037,16 @@
         <v>118</v>
       </c>
       <c r="B38" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>499</v>
+      </c>
+      <c r="I38" s="9" t="s">
         <v>495</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>500</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>501</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="34" x14ac:dyDescent="0.2">
@@ -7054,16 +7054,16 @@
         <v>148</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -7071,13 +7071,13 @@
         <v>96</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
   </sheetData>
@@ -7829,90 +7829,90 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
+        <v>372</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>374</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>376</v>
-      </c>
       <c r="C5" s="15" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -7920,299 +7920,299 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
+        <v>453</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>455</v>
       </c>
-      <c r="B28" s="15" t="s">
-        <v>457</v>
-      </c>
       <c r="C28" s="15" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B44" s="15" t="s">
         <v>118</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -8243,12 +8243,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.5" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" customWidth="1"/>
+    <col min="1" max="1" width="65.5" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
@@ -8278,20 +8280,20 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>368</v>
+        <v>522</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>369</v>
+        <v>521</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2007071600</v>
+        <v>2007161408</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F2" s="17" t="s">
         <v>29</v>
@@ -8877,7 +8879,7 @@
       <c r="AC17" s="43"/>
       <c r="AD17" s="43"/>
     </row>
-    <row r="18" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
         <v>102</v>
       </c>

</xml_diff>